<commit_message>
Working on batching in lvl 4 inputs. Doesn't break but may not be aggregating correctly.
</commit_message>
<xml_diff>
--- a/input/extension/user-defined-energy/TEST-instructions.xlsx
+++ b/input/extension/user-defined-energy/TEST-instructions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="16340" windowHeight="17440" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="16340" windowHeight="17440" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Interpolation_instructions" sheetId="1" r:id="rId1"/>
@@ -60,9 +60,6 @@
     <t>matching_file_name</t>
   </si>
   <si>
-    <t>match_to_trend</t>
-  </si>
-  <si>
     <t>priority</t>
   </si>
   <si>
@@ -90,13 +87,16 @@
     <t>1A1a_Electricity-autoproducer</t>
   </si>
   <si>
-    <t>1A1a_Heat-production</t>
-  </si>
-  <si>
-    <t>1A1bc_Other-transformation</t>
-  </si>
-  <si>
     <t>deu</t>
+  </si>
+  <si>
+    <t>hard_coal</t>
+  </si>
+  <si>
+    <t>brown_coal</t>
+  </si>
+  <si>
+    <t>linear</t>
   </si>
 </sst>
 </file>
@@ -420,8 +420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -454,7 +454,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -475,7 +475,7 @@
         <v>8</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -487,11 +487,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -510,56 +513,56 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>15</v>
-      </c>
-      <c r="J1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2">
         <v>1931</v>
       </c>
       <c r="E2">
-        <v>1936</v>
+        <v>1934</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D3">
-        <v>1931</v>
+        <v>1932</v>
       </c>
       <c r="E3">
         <v>1936</v>
@@ -568,18 +571,18 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D4">
         <v>1931</v>
@@ -591,18 +594,18 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D5">
         <v>1931</v>
@@ -614,7 +617,7 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated style and spacing
</commit_message>
<xml_diff>
--- a/input/extension/user-defined-energy/TEST-instructions.xlsx
+++ b/input/extension/user-defined-energy/TEST-instructions.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
   <si>
     <t>iso</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>linear</t>
+  </si>
+  <si>
+    <t>override_normalization</t>
   </si>
 </sst>
 </file>
@@ -421,7 +424,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -485,18 +488,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -527,8 +531,11 @@
       <c r="J1" t="s">
         <v>15</v>
       </c>
+      <c r="K1" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -551,7 +558,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -574,7 +581,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -597,7 +604,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -614,7 +621,7 @@
         <v>1936</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J5" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Added user option for defining continuity
</commit_message>
<xml_diff>
--- a/input/extension/user-defined-energy/TEST-instructions.xlsx
+++ b/input/extension/user-defined-energy/TEST-instructions.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
   <si>
     <t>iso</t>
   </si>
@@ -100,6 +100,15 @@
   </si>
   <si>
     <t>override_normalization</t>
+  </si>
+  <si>
+    <t>start_continuity</t>
+  </si>
+  <si>
+    <t>end_continuity</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
@@ -488,19 +497,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -534,8 +544,14 @@
       <c r="K1" t="s">
         <v>24</v>
       </c>
+      <c r="L1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -557,8 +573,14 @@
       <c r="J2" t="s">
         <v>17</v>
       </c>
+      <c r="L2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -580,8 +602,14 @@
       <c r="J3" t="s">
         <v>17</v>
       </c>
+      <c r="L3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -603,8 +631,14 @@
       <c r="J4" t="s">
         <v>17</v>
       </c>
+      <c r="L4" t="s">
+        <v>27</v>
+      </c>
+      <c r="M4" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -625,6 +659,12 @@
       </c>
       <c r="J5" t="s">
         <v>17</v>
+      </c>
+      <c r="L5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added instruction sorting, made interpolation files optional
</commit_message>
<xml_diff>
--- a/input/extension/user-defined-energy/TEST-instructions.xlsx
+++ b/input/extension/user-defined-energy/TEST-instructions.xlsx
@@ -9,11 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16340" windowHeight="17440" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="16340" windowHeight="17440" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Interpolation_instructions" sheetId="1" r:id="rId1"/>
-    <sheet name="Trend_instructions" sheetId="2" r:id="rId2"/>
+    <sheet name="Trend_instructions" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
   <si>
     <t>iso</t>
   </si>
@@ -33,70 +32,49 @@
     <t>CEDS_fuel</t>
   </si>
   <si>
+    <t>start_year</t>
+  </si>
+  <si>
+    <t>end_year</t>
+  </si>
+  <si>
+    <t>priority</t>
+  </si>
+  <si>
+    <t>coal_coke</t>
+  </si>
+  <si>
+    <t>deu</t>
+  </si>
+  <si>
+    <t>hard_coal</t>
+  </si>
+  <si>
+    <t>brown_coal</t>
+  </si>
+  <si>
+    <t>override_normalization</t>
+  </si>
+  <si>
+    <t>start_continuity</t>
+  </si>
+  <si>
+    <t>end_continuity</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>user_pct_breakdowns</t>
+  </si>
+  <si>
     <t>CEDS_sector</t>
   </si>
   <si>
-    <t>start_year</t>
-  </si>
-  <si>
-    <t>end_year</t>
-  </si>
-  <si>
-    <t>domain</t>
-  </si>
-  <si>
-    <t>method</t>
-  </si>
-  <si>
-    <t>all</t>
-  </si>
-  <si>
-    <t>EXT_IN</t>
-  </si>
-  <si>
-    <t>TEST4</t>
-  </si>
-  <si>
-    <t>matching_file_name</t>
-  </si>
-  <si>
-    <t>priority</t>
-  </si>
-  <si>
-    <t>coal_coke</t>
-  </si>
-  <si>
     <t>1A1a_Electricity-public</t>
   </si>
   <si>
     <t>1A1a_Electricity-autoproducer</t>
-  </si>
-  <si>
-    <t>deu</t>
-  </si>
-  <si>
-    <t>hard_coal</t>
-  </si>
-  <si>
-    <t>brown_coal</t>
-  </si>
-  <si>
-    <t>linear</t>
-  </si>
-  <si>
-    <t>override_normalization</t>
-  </si>
-  <si>
-    <t>start_continuity</t>
-  </si>
-  <si>
-    <t>end_continuity</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>user_pct_breakdowns</t>
   </si>
 </sst>
 </file>
@@ -418,77 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2">
-        <v>1931</v>
-      </c>
-      <c r="E2">
-        <v>1936</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -506,39 +417,39 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" t="s">
-        <v>21</v>
-      </c>
       <c r="J1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="D2">
         <v>1931</v>
@@ -550,21 +461,21 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="I2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="D3">
         <v>1932</v>
@@ -576,21 +487,21 @@
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="I3" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="D4">
         <v>1931</v>
@@ -602,21 +513,21 @@
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="I4" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D5">
         <v>1931</v>
@@ -628,10 +539,10 @@
         <v>2</v>
       </c>
       <c r="H5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="I5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>